<commit_message>
Updated BOM IC price.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/github_prjs/EmbeddedNeuromophicCamera_PADS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD_project\Neuromophic Camera\pcb and schematics\embedded neuromophic camera\EmbeddedNeuromophicCamera_PADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17216490-413F-944F-98E3-439278CECCEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D058900-2A8F-472D-B316-C1185B9C4AF4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8EA9F011-AF60-47FB-BBDE-C3F1296126CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{8EA9F011-AF60-47FB-BBDE-C3F1296126CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="437">
   <si>
     <t>Name</t>
   </si>
@@ -1409,10 +1409,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1730,27 +1730,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED008CBA-9651-4434-9CA4-378A54734DD1}">
   <dimension ref="A1:G281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A265" sqref="A265:XFD265"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>89</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>90</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>94</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>95</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>96</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>97</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>98</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>99</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>104</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>105</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>106</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>109</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>111</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>112</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>113</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>114</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>115</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>116</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>117</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>119</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>120</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>121</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>123</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>124</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>125</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>127</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>128</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>129</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>130</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>131</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>132</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>133</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>134</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>135</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>136</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>137</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>138</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>139</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>140</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>141</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>142</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>144</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>145</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>146</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>147</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>148</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>150</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>152</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>153</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>154</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>158</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>164</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>167</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>168</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>171</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>174</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>175</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>176</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>177</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>178</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>179</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>182</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>186</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>187</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>190</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>193</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>196</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>199</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>203</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>204</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>205</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>206</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>209</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>210</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>211</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>212</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>213</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>214</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>217</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>220</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>221</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>224</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>227</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>230</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>234</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>235</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>239</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>242</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>246</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>250</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>251</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>252</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>255</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>256</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>257</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>258</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>259</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>260</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>261</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>262</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>263</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>264</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>265</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>266</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>267</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>268</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>269</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>270</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>271</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>272</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>273</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>274</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>275</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>276</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>277</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>278</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>279</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>280</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>281</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>282</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>283</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>284</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>285</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>286</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>287</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>288</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>289</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>290</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>291</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>292</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>293</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>294</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>295</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>296</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>297</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>298</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>299</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>300</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>301</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>302</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>303</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>304</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>305</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>306</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>307</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>308</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>311</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>312</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>313</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>314</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>315</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>316</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>317</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>318</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>319</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>322</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>323</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>324</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>325</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>327</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>328</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>329</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>330</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>331</v>
       </c>
@@ -7412,7 +7412,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>332</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>333</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>334</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>335</v>
       </c>
@@ -7491,7 +7491,7 @@
       <c r="C260" t="s">
         <v>337</v>
       </c>
-      <c r="D260" s="5"/>
+      <c r="D260" s="4"/>
       <c r="E260" t="s">
         <v>14</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>338</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>341</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>342</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>343</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>344</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>348</v>
       </c>
@@ -7625,7 +7625,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>352</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>356</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>359</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>360</v>
       </c>
@@ -7705,7 +7705,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>363</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>364</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>367</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>370</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>373</v>
       </c>
@@ -7805,7 +7805,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>376</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>379</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>382</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>386</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="281" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>388</v>
       </c>
@@ -7899,30 +7899,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A830F9-959C-B34F-BCA6-4F4F23785374}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -7973,8 +7973,11 @@
       <c r="H3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>348</v>
       </c>
@@ -7996,8 +7999,11 @@
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>348</v>
       </c>
@@ -8019,8 +8025,11 @@
       <c r="H5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>348</v>
       </c>
@@ -8042,8 +8051,11 @@
       <c r="H6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>352</v>
       </c>
@@ -8065,8 +8077,11 @@
       <c r="H7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>356</v>
       </c>
@@ -8088,8 +8103,11 @@
       <c r="H8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>360</v>
       </c>
@@ -8111,8 +8129,11 @@
       <c r="H9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -8134,8 +8155,11 @@
       <c r="H10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>367</v>
       </c>
@@ -8158,7 +8182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>370</v>
       </c>
@@ -8180,8 +8204,11 @@
       <c r="H12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>373</v>
       </c>
@@ -8203,8 +8230,11 @@
       <c r="H13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>382</v>
       </c>
@@ -8226,8 +8256,11 @@
       <c r="H14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>386</v>
       </c>
@@ -8249,8 +8282,11 @@
       <c r="H15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>344</v>
       </c>
@@ -8274,6 +8310,32 @@
       </c>
       <c r="H16">
         <v>50</v>
+      </c>
+      <c r="I16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>405</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -8289,17 +8351,17 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>398</v>
       </c>
@@ -8308,7 +8370,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8337,7 +8399,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8360,7 +8422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8383,7 +8445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>379</v>
       </c>
@@ -8406,7 +8468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>376</v>
       </c>

</xml_diff>

<commit_message>
Fixed IN5822 footprint error in BOM.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/github_prjs/EmbeddedNeuromophicCamera_PADS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39C8A68-8338-CE45-8A3F-6AE817A93FD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4CF1D4-165E-9E4B-8E50-B19E67C8F663}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{8EA9F011-AF60-47FB-BBDE-C3F1296126CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="486">
   <si>
     <t xml:space="preserve"> Part Report bom for main_pads.pcb on 2/26/2019 10:16:17</t>
   </si>
@@ -1531,6 +1531,9 @@
   </si>
   <si>
     <t>CLK_33.3M</t>
+  </si>
+  <si>
+    <t>SS34/SMA</t>
   </si>
 </sst>
 </file>
@@ -1699,12 +1702,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1713,6 +1710,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8930,8 +8933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A830F9-959C-B34F-BCA6-4F4F23785374}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8941,16 +8944,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -9283,23 +9286,23 @@
       <c r="A14" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>481</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>482</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="17">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="E14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="15">
         <v>5</v>
       </c>
       <c r="I14" s="6">
@@ -9428,17 +9431,17 @@
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
@@ -10438,17 +10441,17 @@
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="16" t="s">
         <v>452</v>
       </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
@@ -10516,7 +10519,7 @@
         <v>177</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>178</v>
+        <v>485</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>179</v>
@@ -10576,17 +10579,17 @@
       <c r="I61" s="6"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="16" t="s">
         <v>453</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
@@ -10823,19 +10826,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="44" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">

</xml_diff>